<commit_message>
monitoring submodule to 0.6.0
</commit_message>
<xml_diff>
--- a/odk_template_form/ODK-Form-GeoNature-monitoring_template.xlsx
+++ b/odk_template_form/ODK-Form-GeoNature-monitoring_template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="244">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -121,7 +121,7 @@
 Avec les contributions de la **communauté ODK** sur [le forum d’ODK](https://forum.getodk.org).</t>
   </si>
   <si>
-    <t xml:space="preserve">img.png</t>
+    <t xml:space="preserve">logo.png</t>
   </si>
   <si>
     <t xml:space="preserve">Permet de choisir la méthode de sélection du site à renseigner</t>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">begin repeat</t>
   </si>
   <si>
-    <t xml:space="preserve">observers</t>
+    <t xml:space="preserve">observer</t>
   </si>
   <si>
     <t xml:space="preserve">Observat.eur.rice.s</t>
@@ -347,7 +347,7 @@
     <t xml:space="preserve">Boucle pour renseigner l(es) observation(s)</t>
   </si>
   <si>
-    <t xml:space="preserve">observations</t>
+    <t xml:space="preserve">observation</t>
   </si>
   <si>
     <t xml:space="preserve">Espèce(s) observées</t>
@@ -645,7 +645,7 @@
     <t xml:space="preserve">geonature_template_one_repeat_obs_v2</t>
   </si>
   <si>
-    <t xml:space="preserve">3.3</t>
+    <t xml:space="preserve">3.1</t>
   </si>
   <si>
     <t xml:space="preserve">yes</t>
@@ -727,9 +727,6 @@
   </si>
   <si>
     <t xml:space="preserve">visit.observer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">observer</t>
   </si>
   <si>
     <t xml:space="preserve">Nom de la boucle</t>
@@ -749,9 +746,6 @@
   <si>
     <t xml:space="preserve">Valeur = t_datasets.id_dataset
 Choix de remplir par concepteur formulaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">observation</t>
   </si>
   <si>
     <t xml:space="preserve">Valeur = taxref.cd_nom</t>
@@ -989,7 +983,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1014,6 +1008,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1046,10 +1044,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1167,6 +1173,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1336,35 +1346,35 @@
   <dimension ref="A1:U58"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="S8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="S1" activeCellId="0" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="S8" activeCellId="0" sqref="S8"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="V2" activeCellId="0" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="42.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="32.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="62.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="65.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="65.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="40.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="46.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="46.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="47.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="17.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="31.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="39.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="33.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="24.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="28.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="29.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="47.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="28.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="23.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="65.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="23.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="2" width="65.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,164 +1601,172 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7" t="n">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="60.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="B14" s="6"/>
       <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>39</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6" t="s">
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6" t="s">
+      <c r="M14" s="7"/>
+      <c r="N14" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
       <c r="R14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="59.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
@@ -1766,7 +1784,7 @@
       <c r="L15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="N15" s="6" t="s">
+      <c r="N15" s="7" t="s">
         <v>48</v>
       </c>
       <c r="R15" s="2" t="s">
@@ -1774,31 +1792,31 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
@@ -1807,7 +1825,7 @@
       <c r="C19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -1827,7 +1845,7 @@
       <c r="C20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="10" t="s">
         <v>58</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1841,37 +1859,37 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7" t="n">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7" t="s">
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
@@ -1880,7 +1898,7 @@
       <c r="C23" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="10" t="s">
         <v>65</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -1900,7 +1918,7 @@
       <c r="C24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="10" t="s">
         <v>70</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -1917,37 +1935,37 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="10" t="n">
+      <c r="B25" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="12" t="s">
         <v>74</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="57" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -1956,7 +1974,7 @@
       <c r="C26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="10" t="s">
         <v>79</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -1970,58 +1988,58 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12" t="s">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="12"/>
-      <c r="R27" s="12"/>
-      <c r="S27" s="12"/>
-      <c r="T27" s="12"/>
-      <c r="U27" s="12"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
@@ -2030,7 +2048,7 @@
       <c r="C31" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="10" t="s">
         <v>86</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -2040,37 +2058,39 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D32" s="15"/>
+    </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7" t="n">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14" t="s">
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="7"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="7"/>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8"/>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="U34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="69" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
@@ -2079,7 +2099,7 @@
       <c r="C35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="9" t="s">
+      <c r="D35" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -2091,7 +2111,7 @@
       <c r="L35" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="N35" s="6"/>
+      <c r="N35" s="17"/>
       <c r="R35" s="2" t="s">
         <v>96</v>
       </c>
@@ -2100,174 +2120,178 @@
       <c r="A36" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6" t="s">
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
-      <c r="U36" s="6"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="17"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8" t="s">
+      <c r="A37" s="9"/>
+      <c r="B37" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="8"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N38" s="6"/>
+      <c r="N38" s="17"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N39" s="6"/>
+      <c r="N39" s="17"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B40" s="10" t="n">
+      <c r="B40" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="C40" s="17" t="s">
+      <c r="C40" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="E40" s="10" t="s">
+      <c r="E40" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="10"/>
-      <c r="M40" s="10"/>
-      <c r="N40" s="10"/>
-      <c r="O40" s="10"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="10"/>
-      <c r="R40" s="10"/>
-      <c r="S40" s="10"/>
-      <c r="T40" s="10"/>
-      <c r="U40" s="10"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="20"/>
+      <c r="J40" s="20"/>
+      <c r="K40" s="20"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="T40" s="11"/>
+      <c r="U40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1"/>
-      <c r="S41" s="1"/>
-      <c r="T41" s="1"/>
-      <c r="U41" s="1"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+      <c r="U41" s="6"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1"/>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+      <c r="T42" s="6"/>
+      <c r="U42" s="6"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7" t="n">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D43" s="19" t="s">
+      <c r="D43" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="E43" s="19" t="s">
+      <c r="E43" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="19"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
-      <c r="L43" s="7" t="s">
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="7"/>
-      <c r="S43" s="7"/>
-      <c r="T43" s="7"/>
-      <c r="U43" s="7"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="8"/>
+      <c r="O43" s="8"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="8"/>
+      <c r="R43" s="8"/>
+      <c r="S43" s="8"/>
+      <c r="T43" s="8"/>
+      <c r="U43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
@@ -2276,7 +2300,7 @@
       <c r="C44" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D44" s="23" t="s">
         <v>111</v>
       </c>
       <c r="E44" s="5" t="s">
@@ -2296,31 +2320,31 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8" t="s">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="21"/>
-      <c r="M45" s="8"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="8"/>
-      <c r="S45" s="8"/>
-      <c r="T45" s="8"/>
-      <c r="U45" s="8"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="9"/>
+      <c r="R45" s="9"/>
+      <c r="S45" s="9"/>
+      <c r="T45" s="9"/>
+      <c r="U45" s="9"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
@@ -2385,37 +2409,37 @@
       <c r="U50" s="5"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7" t="n">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="D51" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="E51" s="19" t="s">
+      <c r="E51" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="19"/>
-      <c r="L51" s="7" t="s">
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7"/>
-      <c r="Q51" s="7"/>
-      <c r="R51" s="7"/>
-      <c r="S51" s="7"/>
-      <c r="T51" s="7"/>
-      <c r="U51" s="7"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="8"/>
+      <c r="Q51" s="8"/>
+      <c r="R51" s="8"/>
+      <c r="S51" s="8"/>
+      <c r="T51" s="8"/>
+      <c r="U51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -2424,7 +2448,7 @@
       <c r="C52" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D52" s="20" t="s">
+      <c r="D52" s="23" t="s">
         <v>121</v>
       </c>
       <c r="E52" s="5" t="s">
@@ -2441,31 +2465,31 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8" t="s">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
-      <c r="K53" s="21"/>
-      <c r="L53" s="21"/>
-      <c r="M53" s="8"/>
-      <c r="N53" s="8"/>
-      <c r="O53" s="8"/>
-      <c r="P53" s="8"/>
-      <c r="Q53" s="8"/>
-      <c r="R53" s="8"/>
-      <c r="S53" s="8"/>
-      <c r="T53" s="8"/>
-      <c r="U53" s="8"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="24"/>
+      <c r="L53" s="24"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="9"/>
+      <c r="R53" s="9"/>
+      <c r="S53" s="9"/>
+      <c r="T53" s="9"/>
+      <c r="U53" s="9"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="5"/>
@@ -2498,7 +2522,7 @@
       <c r="C56" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D56" s="20" t="s">
+      <c r="D56" s="23" t="s">
         <v>125</v>
       </c>
       <c r="E56" s="5" t="s">
@@ -2528,31 +2552,31 @@
       <c r="L57" s="5"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="12"/>
-      <c r="B58" s="12" t="s">
+      <c r="A58" s="13"/>
+      <c r="B58" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="C58" s="22" t="s">
+      <c r="C58" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="D58" s="22"/>
-      <c r="E58" s="22"/>
-      <c r="F58" s="22"/>
-      <c r="G58" s="22"/>
-      <c r="H58" s="22"/>
-      <c r="I58" s="22"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="22"/>
-      <c r="M58" s="12"/>
-      <c r="N58" s="12"/>
-      <c r="O58" s="12"/>
-      <c r="P58" s="12"/>
-      <c r="Q58" s="12"/>
-      <c r="R58" s="12"/>
-      <c r="S58" s="12"/>
-      <c r="T58" s="12"/>
-      <c r="U58" s="12"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="25"/>
+      <c r="H58" s="25"/>
+      <c r="I58" s="25"/>
+      <c r="J58" s="25"/>
+      <c r="K58" s="25"/>
+      <c r="L58" s="25"/>
+      <c r="M58" s="13"/>
+      <c r="N58" s="13"/>
+      <c r="O58" s="13"/>
+      <c r="P58" s="13"/>
+      <c r="Q58" s="13"/>
+      <c r="R58" s="13"/>
+      <c r="S58" s="13"/>
+      <c r="T58" s="13"/>
+      <c r="U58" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:U58"/>
@@ -2578,35 +2602,35 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.45"/>
   </cols>
   <sheetData>
-    <row r="1" s="24" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="23" t="s">
+    <row r="1" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="26" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+    <row r="2" s="30" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2632,278 +2656,278 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="28" t="s">
+    <row r="7" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="31" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="28" t="s">
+      <c r="D7" s="31"/>
+    </row>
+    <row r="8" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="28"/>
-    </row>
-    <row r="10" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="28" t="s">
+      <c r="D8" s="31"/>
+    </row>
+    <row r="10" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="32" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="28" t="s">
+    <row r="11" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="31" t="s">
         <v>144</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="31" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="12" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="28" t="s">
+    <row r="12" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="31" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="13" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="28" t="s">
+    <row r="13" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="31" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="14" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-    </row>
-    <row r="15" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="28" t="s">
+    <row r="14" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+    </row>
+    <row r="15" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="32" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="16" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28" t="s">
+    <row r="16" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="31" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="17" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28" t="s">
+    <row r="17" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="31" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="28" t="s">
+    <row r="18" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="31" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="19" s="24" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="29"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-    </row>
-    <row r="20" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28" t="s">
+    <row r="19" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="32"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+    </row>
+    <row r="20" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="32" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="21" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="28" t="s">
+    <row r="21" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="31" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="22" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28" t="s">
+    <row r="22" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="31" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="23" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="28" t="s">
+    <row r="23" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="31" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="24" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
-      <c r="C24" s="28"/>
-    </row>
-    <row r="25" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="28" t="s">
+    <row r="24" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+    </row>
+    <row r="25" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="31" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="26" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="28" t="s">
+    <row r="26" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="32" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="27" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="28" t="s">
+    <row r="27" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="31" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="28" s="29" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="28" t="s">
+    <row r="28" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="31" t="s">
         <v>164</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="31" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="29" s="24" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-    </row>
-    <row r="30" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="30" t="s">
+    <row r="29" s="27" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+    </row>
+    <row r="30" s="35" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="34" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="31" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="30" t="s">
+    <row r="31" s="35" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="34" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="32" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="30" t="s">
+    <row r="32" s="35" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="34" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="33" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="30" t="s">
+    <row r="33" s="35" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="34" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="34" s="32" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="30" t="s">
+    <row r="34" s="35" customFormat="true" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="C34" s="31" t="s">
+      <c r="C34" s="34" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2939,10 +2963,10 @@
       <c r="A39" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C39" s="33" t="s">
+      <c r="C39" s="36" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2950,10 +2974,10 @@
       <c r="A40" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B40" s="33" t="s">
+      <c r="B40" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="C40" s="33" t="s">
+      <c r="C40" s="36" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2961,10 +2985,10 @@
       <c r="A41" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="C41" s="33" t="s">
+      <c r="C41" s="36" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2972,10 +2996,10 @@
       <c r="A42" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="C42" s="33" t="s">
+      <c r="C42" s="36" t="s">
         <v>191</v>
       </c>
     </row>
@@ -2983,10 +3007,10 @@
       <c r="A43" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="36" t="s">
         <v>192</v>
       </c>
     </row>
@@ -2994,10 +3018,10 @@
       <c r="A44" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="C44" s="33" t="s">
+      <c r="C44" s="36" t="s">
         <v>193</v>
       </c>
     </row>
@@ -3005,10 +3029,10 @@
       <c r="A45" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B45" s="33" t="s">
+      <c r="B45" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C45" s="33" t="s">
+      <c r="C45" s="36" t="s">
         <v>194</v>
       </c>
     </row>
@@ -3016,10 +3040,10 @@
       <c r="A46" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B46" s="33" t="s">
+      <c r="B46" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="C46" s="33" t="s">
+      <c r="C46" s="36" t="s">
         <v>195</v>
       </c>
     </row>
@@ -3045,7 +3069,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.89"/>
@@ -3055,34 +3079,34 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="39" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="40" t="s">
         <v>203</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36" t="s">
+      <c r="D2" s="39"/>
+      <c r="E2" s="39" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3112,361 +3136,361 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="38" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="39" width="28.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="39" width="17.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="9.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="39" width="18.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="39" width="44.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="39" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="41" width="14.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="42" width="29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="42" width="17.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="42" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="42" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="42" width="44.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="42" width="11.55"/>
   </cols>
   <sheetData>
-    <row r="1" s="38" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40" t="s">
+    <row r="1" s="41" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="43" t="s">
         <v>205</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="43" t="s">
         <v>206</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="43" t="s">
         <v>207</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="43" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="2" s="38" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
+    <row r="2" s="41" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43" t="s">
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="42" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44" t="s">
+      <c r="C4" s="47"/>
+      <c r="D4" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="42" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="42" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="D7" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="42" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="48" t="s">
         <v>210</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45" t="s">
+      <c r="C8" s="49"/>
+      <c r="D8" s="49" t="s">
         <v>215</v>
       </c>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45" t="s">
+      <c r="E8" s="49"/>
+      <c r="F8" s="49" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="42" t="s">
         <v>221</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="42" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="42" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="D11" s="39" t="s">
+      <c r="D11" s="42" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="42" t="s">
         <v>227</v>
       </c>
-      <c r="D12" s="39" t="s">
+      <c r="D12" s="42" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="42" t="s">
         <v>228</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="42" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="B14" s="39" t="s">
+      <c r="B14" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="D14" s="39" t="s">
+      <c r="D14" s="42" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="D15" s="39" t="s">
+      <c r="D15" s="42" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47" t="s">
         <v>231</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="44" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="41" t="s">
+      <c r="B17" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="B17" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="44" t="s">
+      <c r="D17" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47" t="s">
         <v>234</v>
       </c>
-      <c r="D17" s="44" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="B19" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+    </row>
+    <row r="21" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47" t="s">
         <v>215</v>
       </c>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="B18" s="42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44" t="s">
-        <v>222</v>
-      </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44" t="s">
-        <v>222</v>
-      </c>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44" t="s">
+      <c r="E21" s="47" t="n">
+        <v>99999</v>
+      </c>
+      <c r="F21" s="50" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44" t="s">
+    <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="47"/>
+      <c r="D22" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+    </row>
+    <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="44"/>
-      <c r="F20" s="44"/>
-    </row>
-    <row r="21" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44" t="s">
-        <v>215</v>
-      </c>
-      <c r="E21" s="44" t="n">
-        <v>99999</v>
-      </c>
-      <c r="F21" s="46" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41" t="s">
-        <v>233</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="44" t="s">
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+    </row>
+    <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="45" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47" t="s">
         <v>224</v>
       </c>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-    </row>
-    <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41" t="s">
-        <v>238</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44" t="s">
-        <v>215</v>
-      </c>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="41" t="s">
-        <v>238</v>
-      </c>
-      <c r="B24" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-    </row>
-    <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41" t="s">
-        <v>238</v>
-      </c>
-      <c r="B25" s="42" t="s">
-        <v>125</v>
-      </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44" t="s">
-        <v>224</v>
-      </c>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3490,7 +3514,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3517,147 +3541,147 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.4453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="47" width="103.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="47" width="47.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="48" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="47" width="46.66"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="7" style="48" width="9.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="47" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="51" width="11.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="51" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="51" width="103.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="51" width="47.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="52" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="51" width="46.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="7" style="52" width="9.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="51" width="11.55"/>
   </cols>
   <sheetData>
-    <row r="1" s="49" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="49" t="s">
+    <row r="1" s="53" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="53" t="s">
+        <v>238</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="53" t="s">
         <v>240</v>
       </c>
-      <c r="B1" s="49" t="s">
-        <v>222</v>
-      </c>
-      <c r="C1" s="49" t="s">
+      <c r="E1" s="53" t="s">
         <v>241</v>
       </c>
-      <c r="D1" s="49" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="51" t="s">
         <v>242</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="B2" s="54" t="n">
+        <v>44904</v>
+      </c>
+      <c r="C2" s="51" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="47" t="s">
-        <v>244</v>
-      </c>
-      <c r="B2" s="50" t="n">
-        <v>44904</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>245</v>
-      </c>
-    </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="50"/>
+      <c r="B3" s="54"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="50"/>
+      <c r="B4" s="54"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="50"/>
+      <c r="B5" s="54"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="50"/>
+      <c r="B6" s="54"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="50"/>
+      <c r="B8" s="54"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="50"/>
+      <c r="B9" s="54"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="50"/>
+      <c r="B10" s="54"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="50"/>
+      <c r="B11" s="54"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="50"/>
+      <c r="B12" s="54"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="50"/>
+      <c r="B13" s="54"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="50"/>
+      <c r="B14" s="54"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="50"/>
+      <c r="B15" s="54"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="50"/>
+      <c r="B16" s="54"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="50"/>
+      <c r="B17" s="54"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="50"/>
+      <c r="B18" s="54"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="50"/>
+      <c r="B19" s="54"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="50"/>
+      <c r="B20" s="54"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="50"/>
+      <c r="B21" s="54"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="50"/>
+      <c r="B22" s="54"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="50"/>
+      <c r="B23" s="54"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="50"/>
+      <c r="B24" s="54"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="50"/>
+      <c r="B25" s="54"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="50"/>
+      <c r="B26" s="54"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="50"/>
+      <c r="B27" s="54"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="50"/>
+      <c r="B28" s="54"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="50"/>
+      <c r="B29" s="54"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="50"/>
+      <c r="B30" s="54"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="50"/>
+      <c r="B31" s="54"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="50"/>
+      <c r="B32" s="54"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="50"/>
+      <c r="B33" s="54"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="50"/>
+      <c r="B34" s="54"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="50"/>
+      <c r="B35" s="54"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="50"/>
-      <c r="C36" s="51"/>
+      <c r="B36" s="54"/>
+      <c r="C36" s="55"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>